<commit_message>
Add timeline feature, cluster options, fix legends, edit data to include properly formated dates
</commit_message>
<xml_diff>
--- a/GreekData.xlsx
+++ b/GreekData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="384">
   <si>
     <t>Name</t>
   </si>
@@ -428,6 +428,9 @@
     <t>http://epigraphy.packhum.org/text/435?&amp;bookid=4&amp;location=7</t>
   </si>
   <si>
+    <t>411</t>
+  </si>
+  <si>
     <t>http://clas-lgpn2.classics.ox.ac.uk/cgi-bin/lgpn_search.cgi?id=V2-31162</t>
   </si>
   <si>
@@ -611,9 +614,15 @@
     <t>http://epigraphy.packhum.org/text/344307</t>
   </si>
   <si>
+    <t>500</t>
+  </si>
+  <si>
     <t>http://clas-lgpn2.classics.ox.ac.uk/cgi-bin/lgpn_search.cgi?id=V1-45735&amp;style=</t>
   </si>
   <si>
+    <t>350</t>
+  </si>
+  <si>
     <t>http://epigraphy.packhum.org/text/344025?hs=4633-4645</t>
   </si>
   <si>
@@ -629,6 +638,9 @@
     <t>36.0913, 28.0882</t>
   </si>
   <si>
+    <t>200</t>
+  </si>
+  <si>
     <t>Dodecanese</t>
   </si>
   <si>
@@ -686,6 +698,9 @@
     <t>37.2336, 25.1616</t>
   </si>
   <si>
+    <t>192</t>
+  </si>
+  <si>
     <t>Cyclades</t>
   </si>
   <si>
@@ -830,6 +845,9 @@
     <t>37.3149, 27.1642</t>
   </si>
   <si>
+    <t>405</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ionia </t>
   </si>
   <si>
@@ -921,6 +939,9 @@
   </si>
   <si>
     <t>40.4257, 27.0671</t>
+  </si>
+  <si>
+    <t>208</t>
   </si>
   <si>
     <t>http://clas-lgpn2.classics.ox.ac.uk/cgi-bin/lgpn_search.cgi?id=V5a-15460&amp;style=</t>
@@ -1529,7 +1550,7 @@
         <v>51</v>
       </c>
       <c r="J9" t="n">
-        <v>200.0</v>
+        <v>250.0</v>
       </c>
       <c r="K9" t="s">
         <v>47</v>
@@ -2627,8 +2648,8 @@
       <c r="H38" t="s">
         <v>135</v>
       </c>
-      <c r="I38" t="n">
-        <v>411.0</v>
+      <c r="I38" t="s">
+        <v>138</v>
       </c>
       <c r="J38" t="n">
         <v>411.0</v>
@@ -2637,7 +2658,7 @@
         <v>70</v>
       </c>
       <c r="L38" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39">
@@ -2666,7 +2687,7 @@
         <v>135</v>
       </c>
       <c r="I39" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J39" t="n">
         <v>413.0</v>
@@ -2675,7 +2696,7 @@
         <v>70</v>
       </c>
       <c r="L39" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40">
@@ -2704,7 +2725,7 @@
         <v>135</v>
       </c>
       <c r="I40" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J40" t="n">
         <v>410.0</v>
@@ -2713,7 +2734,7 @@
         <v>70</v>
       </c>
       <c r="L40" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41">
@@ -2742,7 +2763,7 @@
         <v>62</v>
       </c>
       <c r="I41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J41" t="n">
         <v>400.0</v>
@@ -2751,7 +2772,7 @@
         <v>70</v>
       </c>
       <c r="L41" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42">
@@ -2780,7 +2801,7 @@
         <v>62</v>
       </c>
       <c r="I42" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J42" t="n">
         <v>400.0</v>
@@ -2789,7 +2810,7 @@
         <v>70</v>
       </c>
       <c r="L42" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43">
@@ -2818,7 +2839,7 @@
         <v>62</v>
       </c>
       <c r="I43" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J43" t="n">
         <v>375.0</v>
@@ -2827,7 +2848,7 @@
         <v>70</v>
       </c>
       <c r="L43" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44">
@@ -2841,10 +2862,10 @@
         <v>50</v>
       </c>
       <c r="D44" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E44" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F44" t="n">
         <v>37.7244</v>
@@ -2856,7 +2877,7 @@
         <v>62</v>
       </c>
       <c r="I44" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J44" t="n">
         <v>375.0</v>
@@ -2865,7 +2886,7 @@
         <v>70</v>
       </c>
       <c r="L44" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45">
@@ -2879,10 +2900,10 @@
         <v>50</v>
       </c>
       <c r="D45" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E45" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F45" t="n">
         <v>37.8982</v>
@@ -2903,7 +2924,7 @@
         <v>70</v>
       </c>
       <c r="L45" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46">
@@ -2917,10 +2938,10 @@
         <v>50</v>
       </c>
       <c r="D46" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E46" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F46" t="n">
         <v>37.9719</v>
@@ -2932,7 +2953,7 @@
         <v>62</v>
       </c>
       <c r="I46" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J46" t="n">
         <v>340.0</v>
@@ -2941,7 +2962,7 @@
         <v>70</v>
       </c>
       <c r="L46" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47">
@@ -2955,10 +2976,10 @@
         <v>50</v>
       </c>
       <c r="D47" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E47" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F47" t="n">
         <v>38.0564</v>
@@ -2970,7 +2991,7 @@
         <v>24</v>
       </c>
       <c r="I47" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J47" t="n">
         <v>210.0</v>
@@ -2979,7 +3000,7 @@
         <v>70</v>
       </c>
       <c r="L47" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48">
@@ -2993,7 +3014,7 @@
         <v>50</v>
       </c>
       <c r="D48" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E48" t="s">
         <v>77</v>
@@ -3008,7 +3029,7 @@
         <v>17</v>
       </c>
       <c r="I48" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J48" t="n">
         <v>275.0</v>
@@ -3017,7 +3038,7 @@
         <v>70</v>
       </c>
       <c r="L48" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49">
@@ -3046,7 +3067,7 @@
         <v>36</v>
       </c>
       <c r="I49" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J49" t="n">
         <v>275.0</v>
@@ -3055,7 +3076,7 @@
         <v>70</v>
       </c>
       <c r="L49" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50">
@@ -3093,7 +3114,7 @@
         <v>70</v>
       </c>
       <c r="L50" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51">
@@ -3122,7 +3143,7 @@
         <v>24</v>
       </c>
       <c r="I51" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J51" t="n">
         <v>212.0</v>
@@ -3131,7 +3152,7 @@
         <v>70</v>
       </c>
       <c r="L51" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52">
@@ -3145,10 +3166,10 @@
         <v>50</v>
       </c>
       <c r="D52" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E52" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F52" t="n">
         <v>37.8663</v>
@@ -3160,24 +3181,24 @@
         <v>24</v>
       </c>
       <c r="I52" t="s">
-        <v>172</v>
-      </c>
-      <c r="J52" t="s">
-        <v>172</v>
+        <v>173</v>
+      </c>
+      <c r="J52" t="n">
+        <v>210.0</v>
       </c>
       <c r="K52" t="s">
         <v>70</v>
       </c>
       <c r="L52" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B53" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C53" t="s">
         <v>125</v>
@@ -3198,24 +3219,24 @@
         <v>17</v>
       </c>
       <c r="I53" t="s">
-        <v>175</v>
-      </c>
-      <c r="J53" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="J53" t="n">
+        <v>318.0</v>
       </c>
       <c r="K53" t="s">
         <v>70</v>
       </c>
       <c r="L53" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B54" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C54" t="s">
         <v>125</v>
@@ -3236,16 +3257,16 @@
         <v>17</v>
       </c>
       <c r="I54" t="s">
-        <v>177</v>
-      </c>
-      <c r="J54" t="s">
-        <v>177</v>
+        <v>178</v>
+      </c>
+      <c r="J54" t="n">
+        <v>303.0</v>
       </c>
       <c r="K54" t="s">
         <v>70</v>
       </c>
       <c r="L54" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55">
@@ -3253,13 +3274,13 @@
         <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C55" t="s">
         <v>54</v>
       </c>
       <c r="D55" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E55" t="s">
         <v>77</v>
@@ -3274,16 +3295,16 @@
         <v>135</v>
       </c>
       <c r="I55" t="s">
-        <v>181</v>
-      </c>
-      <c r="J55" t="s">
-        <v>181</v>
+        <v>182</v>
+      </c>
+      <c r="J55" t="n">
+        <v>400.0</v>
       </c>
       <c r="K55" t="s">
         <v>70</v>
       </c>
       <c r="L55" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="56">
@@ -3297,10 +3318,10 @@
         <v>14</v>
       </c>
       <c r="D56" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E56" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F56" t="n">
         <v>39.1341</v>
@@ -3314,31 +3335,31 @@
       <c r="I56" t="s">
         <v>46</v>
       </c>
-      <c r="J56" t="s">
-        <v>46</v>
+      <c r="J56" t="n">
+        <v>100.0</v>
       </c>
       <c r="K56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L56" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B57" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C57" t="s">
         <v>54</v>
       </c>
       <c r="D57" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E57" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F57" t="n">
         <v>38.3764</v>
@@ -3350,16 +3371,16 @@
         <v>135</v>
       </c>
       <c r="I57" t="s">
-        <v>190</v>
-      </c>
-      <c r="J57" t="s">
-        <v>190</v>
+        <v>191</v>
+      </c>
+      <c r="J57" t="n">
+        <v>440.0</v>
       </c>
       <c r="K57" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L57" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="58">
@@ -3373,10 +3394,10 @@
         <v>14</v>
       </c>
       <c r="D58" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E58" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F58" t="n">
         <v>37.695</v>
@@ -3385,19 +3406,19 @@
         <v>26.935</v>
       </c>
       <c r="H58" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I58" t="s">
-        <v>194</v>
-      </c>
-      <c r="J58" t="s">
-        <v>194</v>
+        <v>195</v>
+      </c>
+      <c r="J58" t="n">
+        <v>550.0</v>
       </c>
       <c r="K58" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L58" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="59">
@@ -3411,10 +3432,10 @@
         <v>14</v>
       </c>
       <c r="D59" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E59" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F59" t="n">
         <v>37.695</v>
@@ -3423,19 +3444,19 @@
         <v>26.935</v>
       </c>
       <c r="H59" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I59" t="s">
-        <v>196</v>
-      </c>
-      <c r="J59" t="s">
-        <v>196</v>
+        <v>197</v>
+      </c>
+      <c r="J59" t="n">
+        <v>550.0</v>
       </c>
       <c r="K59" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L59" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60">
@@ -3449,10 +3470,10 @@
         <v>14</v>
       </c>
       <c r="D60" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E60" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F60" t="n">
         <v>37.695</v>
@@ -3461,19 +3482,19 @@
         <v>26.935</v>
       </c>
       <c r="H60" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I60" t="s">
-        <v>196</v>
-      </c>
-      <c r="J60" t="s">
-        <v>196</v>
+        <v>197</v>
+      </c>
+      <c r="J60" t="n">
+        <v>550.0</v>
       </c>
       <c r="K60" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L60" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61">
@@ -3487,10 +3508,10 @@
         <v>14</v>
       </c>
       <c r="D61" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E61" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F61" t="n">
         <v>37.695</v>
@@ -3501,17 +3522,17 @@
       <c r="H61" t="n">
         <v>500.0</v>
       </c>
-      <c r="I61" t="n">
-        <v>500.0</v>
+      <c r="I61" t="s">
+        <v>200</v>
       </c>
       <c r="J61" t="n">
         <v>500.0</v>
       </c>
       <c r="K61" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L61" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62">
@@ -3525,10 +3546,10 @@
         <v>14</v>
       </c>
       <c r="D62" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E62" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F62" t="n">
         <v>37.695</v>
@@ -3539,17 +3560,17 @@
       <c r="H62" t="s">
         <v>62</v>
       </c>
-      <c r="I62" t="n">
-        <v>350.0</v>
+      <c r="I62" t="s">
+        <v>202</v>
       </c>
       <c r="J62" t="n">
         <v>350.0</v>
       </c>
       <c r="K62" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L62" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="63">
@@ -3557,16 +3578,16 @@
         <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C63" t="s">
         <v>54</v>
       </c>
       <c r="D63" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E63" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F63" t="n">
         <v>37.695</v>
@@ -3575,19 +3596,19 @@
         <v>26.935</v>
       </c>
       <c r="H63" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I63" t="s">
-        <v>194</v>
-      </c>
-      <c r="J63" t="s">
-        <v>194</v>
+        <v>195</v>
+      </c>
+      <c r="J63" t="n">
+        <v>550.0</v>
       </c>
       <c r="K63" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L63" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64">
@@ -3601,10 +3622,10 @@
         <v>14</v>
       </c>
       <c r="D64" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E64" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F64" t="n">
         <v>36.0913</v>
@@ -3615,17 +3636,17 @@
       <c r="H64" t="s">
         <v>24</v>
       </c>
-      <c r="I64" t="n">
-        <v>200.0</v>
+      <c r="I64" t="s">
+        <v>208</v>
       </c>
       <c r="J64" t="n">
         <v>200.0</v>
       </c>
       <c r="K64" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="L64" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="65">
@@ -3639,10 +3660,10 @@
         <v>14</v>
       </c>
       <c r="D65" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E65" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F65" t="n">
         <v>36.0913</v>
@@ -3654,16 +3675,16 @@
         <v>24</v>
       </c>
       <c r="I65" t="s">
-        <v>207</v>
-      </c>
-      <c r="J65" t="s">
-        <v>207</v>
+        <v>211</v>
+      </c>
+      <c r="J65" t="n">
+        <v>175.0</v>
       </c>
       <c r="K65" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="L65" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="66">
@@ -3677,10 +3698,10 @@
         <v>14</v>
       </c>
       <c r="D66" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E66" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F66" t="n">
         <v>38.3905</v>
@@ -3692,16 +3713,16 @@
         <v>17</v>
       </c>
       <c r="I66" t="s">
-        <v>211</v>
-      </c>
-      <c r="J66" t="s">
-        <v>211</v>
+        <v>215</v>
+      </c>
+      <c r="J66" t="n">
+        <v>308.0</v>
       </c>
       <c r="K66" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="L66" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="67">
@@ -3715,10 +3736,10 @@
         <v>14</v>
       </c>
       <c r="D67" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="E67" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F67" t="n">
         <v>38.9466</v>
@@ -3732,14 +3753,14 @@
       <c r="I67" t="s">
         <v>51</v>
       </c>
-      <c r="J67" t="s">
-        <v>51</v>
+      <c r="J67" t="n">
+        <v>250.0</v>
       </c>
       <c r="K67" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="L67" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68">
@@ -3753,10 +3774,10 @@
         <v>14</v>
       </c>
       <c r="D68" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="E68" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F68" t="n">
         <v>38.3982</v>
@@ -3770,14 +3791,14 @@
       <c r="I68" t="s">
         <v>37</v>
       </c>
-      <c r="J68" t="s">
-        <v>37</v>
+      <c r="J68" t="n">
+        <v>325.0</v>
       </c>
       <c r="K68" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="L68" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="69">
@@ -3791,10 +3812,10 @@
         <v>14</v>
       </c>
       <c r="D69" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="E69" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F69" t="n">
         <v>38.3982</v>
@@ -3808,14 +3829,14 @@
       <c r="I69" t="s">
         <v>37</v>
       </c>
-      <c r="J69" t="s">
-        <v>37</v>
+      <c r="J69" t="n">
+        <v>325.0</v>
       </c>
       <c r="K69" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="L69" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="70">
@@ -3829,10 +3850,10 @@
         <v>50</v>
       </c>
       <c r="D70" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="E70" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F70" t="n">
         <v>38.3982</v>
@@ -3846,14 +3867,14 @@
       <c r="I70" t="s">
         <v>17</v>
       </c>
-      <c r="J70" t="s">
-        <v>17</v>
+      <c r="J70" t="n">
+        <v>325.0</v>
       </c>
       <c r="K70" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="L70" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="71">
@@ -3867,10 +3888,10 @@
         <v>14</v>
       </c>
       <c r="D71" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="E71" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="F71" t="n">
         <v>37.2336</v>
@@ -3881,17 +3902,17 @@
       <c r="H71" t="s">
         <v>24</v>
       </c>
-      <c r="I71" t="n">
-        <v>192.0</v>
+      <c r="I71" t="s">
+        <v>228</v>
       </c>
       <c r="J71" t="n">
         <v>192.0</v>
       </c>
       <c r="K71" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="L71" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="72">
@@ -3905,10 +3926,10 @@
         <v>14</v>
       </c>
       <c r="D72" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="E72" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F72" t="n">
         <v>37.6167</v>
@@ -3922,14 +3943,14 @@
       <c r="I72" t="s">
         <v>51</v>
       </c>
-      <c r="J72" t="s">
-        <v>51</v>
+      <c r="J72" t="n">
+        <v>250.0</v>
       </c>
       <c r="K72" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="L72" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="73">
@@ -3943,10 +3964,10 @@
         <v>14</v>
       </c>
       <c r="D73" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="E73" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="F73" t="n">
         <v>36.364</v>
@@ -3960,14 +3981,14 @@
       <c r="I73" t="s">
         <v>51</v>
       </c>
-      <c r="J73" t="s">
-        <v>51</v>
+      <c r="J73" t="n">
+        <v>250.0</v>
       </c>
       <c r="K73" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="L73" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="74">
@@ -3981,10 +4002,10 @@
         <v>14</v>
       </c>
       <c r="D74" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E74" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F74" t="n">
         <v>36.744</v>
@@ -3993,19 +4014,19 @@
         <v>24.422</v>
       </c>
       <c r="H74" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="I74" t="s">
-        <v>235</v>
-      </c>
-      <c r="J74" t="s">
-        <v>235</v>
+        <v>240</v>
+      </c>
+      <c r="J74" t="n">
+        <v>350.0</v>
       </c>
       <c r="K74" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="L74" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75">
@@ -4019,10 +4040,10 @@
         <v>14</v>
       </c>
       <c r="D75" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="E75" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="F75" t="n">
         <v>32.493</v>
@@ -4034,16 +4055,16 @@
         <v>62</v>
       </c>
       <c r="I75" t="s">
-        <v>240</v>
-      </c>
-      <c r="J75" t="s">
-        <v>240</v>
+        <v>245</v>
+      </c>
+      <c r="J75" t="n">
+        <v>350.0</v>
       </c>
       <c r="K75" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="L75" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
     </row>
     <row r="76">
@@ -4057,10 +4078,10 @@
         <v>50</v>
       </c>
       <c r="D76" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="E76" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="F76" t="n">
         <v>38.3048</v>
@@ -4074,14 +4095,14 @@
       <c r="I76" t="s">
         <v>24</v>
       </c>
-      <c r="J76" t="s">
-        <v>24</v>
+      <c r="J76" t="n">
+        <v>250.0</v>
       </c>
       <c r="K76" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="L76" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="77">
@@ -4095,10 +4116,10 @@
         <v>14</v>
       </c>
       <c r="D77" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="E77" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="F77" t="n">
         <v>36.562</v>
@@ -4112,14 +4133,14 @@
       <c r="I77" t="s">
         <v>24</v>
       </c>
-      <c r="J77" t="s">
-        <v>24</v>
+      <c r="J77" t="n">
+        <v>250.0</v>
       </c>
       <c r="K77" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="L77" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
     </row>
     <row r="78">
@@ -4133,10 +4154,10 @@
         <v>14</v>
       </c>
       <c r="D78" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="E78" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="F78" t="n">
         <v>37.44</v>
@@ -4148,16 +4169,16 @@
         <v>24</v>
       </c>
       <c r="I78" t="s">
-        <v>253</v>
-      </c>
-      <c r="J78" t="s">
-        <v>253</v>
+        <v>258</v>
+      </c>
+      <c r="J78" t="n">
+        <v>188.0</v>
       </c>
       <c r="K78" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="L78" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="79">
@@ -4171,10 +4192,10 @@
         <v>14</v>
       </c>
       <c r="D79" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="E79" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="F79" t="n">
         <v>37.44</v>
@@ -4188,14 +4209,14 @@
       <c r="I79" t="s">
         <v>51</v>
       </c>
-      <c r="J79" t="s">
-        <v>51</v>
+      <c r="J79" t="n">
+        <v>250.0</v>
       </c>
       <c r="K79" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="L79" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
     </row>
     <row r="80">
@@ -4209,10 +4230,10 @@
         <v>14</v>
       </c>
       <c r="D80" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="E80" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="F80" t="n">
         <v>37.44</v>
@@ -4226,14 +4247,14 @@
       <c r="I80" t="s">
         <v>51</v>
       </c>
-      <c r="J80" t="s">
-        <v>51</v>
+      <c r="J80" t="n">
+        <v>250.0</v>
       </c>
       <c r="K80" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="L80" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="81">
@@ -4247,10 +4268,10 @@
         <v>14</v>
       </c>
       <c r="D81" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="E81" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="F81" t="n">
         <v>37.0216</v>
@@ -4262,16 +4283,16 @@
         <v>24</v>
       </c>
       <c r="I81" t="s">
-        <v>261</v>
-      </c>
-      <c r="J81" t="s">
-        <v>261</v>
+        <v>266</v>
+      </c>
+      <c r="J81" t="n">
+        <v>201.0</v>
       </c>
       <c r="K81" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="L81" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="82">
@@ -4285,10 +4306,10 @@
         <v>14</v>
       </c>
       <c r="D82" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="E82" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="F82" t="n">
         <v>37.0216</v>
@@ -4302,14 +4323,14 @@
       <c r="I82" t="s">
         <v>46</v>
       </c>
-      <c r="J82" t="s">
-        <v>46</v>
+      <c r="J82" t="n">
+        <v>150.0</v>
       </c>
       <c r="K82" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="L82" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="83">
@@ -4323,10 +4344,10 @@
         <v>14</v>
       </c>
       <c r="D83" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="E83" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="F83" t="n">
         <v>38.2259</v>
@@ -4338,16 +4359,16 @@
         <v>24</v>
       </c>
       <c r="I83" t="s">
-        <v>267</v>
-      </c>
-      <c r="J83" t="s">
-        <v>267</v>
+        <v>272</v>
+      </c>
+      <c r="J83" t="n">
+        <v>200.0</v>
       </c>
       <c r="K83" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L83" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
     <row r="84">
@@ -4361,10 +4382,10 @@
         <v>50</v>
       </c>
       <c r="D84" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="E84" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="F84" t="n">
         <v>37.3149</v>
@@ -4375,17 +4396,17 @@
       <c r="H84" t="s">
         <v>135</v>
       </c>
-      <c r="I84" t="n">
-        <v>405.0</v>
+      <c r="I84" t="s">
+        <v>277</v>
       </c>
       <c r="J84" t="n">
         <v>405.0</v>
       </c>
       <c r="K84" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="L84" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="85">
@@ -4399,10 +4420,10 @@
         <v>50</v>
       </c>
       <c r="D85" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="E85" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="F85" t="n">
         <v>37.3149</v>
@@ -4414,16 +4435,16 @@
         <v>24</v>
       </c>
       <c r="I85" t="s">
-        <v>274</v>
-      </c>
-      <c r="J85" t="s">
-        <v>274</v>
+        <v>280</v>
+      </c>
+      <c r="J85" t="n">
+        <v>240.0</v>
       </c>
       <c r="K85" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="L85" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="86">
@@ -4437,10 +4458,10 @@
         <v>50</v>
       </c>
       <c r="D86" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="E86" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="F86" t="n">
         <v>37.3149</v>
@@ -4454,31 +4475,31 @@
       <c r="I86" t="s">
         <v>81</v>
       </c>
-      <c r="J86" t="s">
-        <v>81</v>
+      <c r="J86" t="n">
+        <v>375.0</v>
       </c>
       <c r="K86" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="L86" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B87" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C87" t="s">
         <v>54</v>
       </c>
       <c r="D87" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="E87" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="F87" t="n">
         <v>38.0632</v>
@@ -4490,33 +4511,33 @@
         <v>17</v>
       </c>
       <c r="I87" t="s">
-        <v>279</v>
-      </c>
-      <c r="J87" t="s">
-        <v>279</v>
+        <v>285</v>
+      </c>
+      <c r="J87" t="n">
+        <v>311.0</v>
       </c>
       <c r="K87" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="L87" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B88" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C88" t="s">
         <v>125</v>
       </c>
       <c r="D88" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="E88" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="F88" t="n">
         <v>38.0632</v>
@@ -4528,16 +4549,16 @@
         <v>17</v>
       </c>
       <c r="I88" t="s">
-        <v>279</v>
-      </c>
-      <c r="J88" t="s">
-        <v>279</v>
+        <v>285</v>
+      </c>
+      <c r="J88" t="n">
+        <v>311.0</v>
       </c>
       <c r="K88" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="L88" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="89">
@@ -4551,10 +4572,10 @@
         <v>14</v>
       </c>
       <c r="D89" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="E89" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="F89" t="n">
         <v>38.0632</v>
@@ -4566,16 +4587,16 @@
         <v>17</v>
       </c>
       <c r="I89" t="s">
-        <v>279</v>
-      </c>
-      <c r="J89" t="s">
-        <v>279</v>
+        <v>285</v>
+      </c>
+      <c r="J89" t="n">
+        <v>311.0</v>
       </c>
       <c r="K89" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="L89" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="90">
@@ -4589,10 +4610,10 @@
         <v>14</v>
       </c>
       <c r="D90" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="E90" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="F90" t="n">
         <v>38.0632</v>
@@ -4606,14 +4627,14 @@
       <c r="I90" t="s">
         <v>24</v>
       </c>
-      <c r="J90" t="s">
-        <v>24</v>
+      <c r="J90" t="n">
+        <v>250.0</v>
       </c>
       <c r="K90" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="L90" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="91">
@@ -4627,10 +4648,10 @@
         <v>14</v>
       </c>
       <c r="D91" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="E91" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="F91" t="n">
         <v>38.0632</v>
@@ -4644,14 +4665,14 @@
       <c r="I91" t="s">
         <v>37</v>
       </c>
-      <c r="J91" t="s">
-        <v>37</v>
+      <c r="J91" t="n">
+        <v>325.0</v>
       </c>
       <c r="K91" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="L91" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="92">
@@ -4665,10 +4686,10 @@
         <v>14</v>
       </c>
       <c r="D92" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="E92" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="F92" t="n">
         <v>38.124</v>
@@ -4682,14 +4703,14 @@
       <c r="I92" t="s">
         <v>46</v>
       </c>
-      <c r="J92" t="s">
-        <v>46</v>
+      <c r="J92" t="n">
+        <v>150.0</v>
       </c>
       <c r="K92" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="L92" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="93">
@@ -4703,10 +4724,10 @@
         <v>14</v>
       </c>
       <c r="D93" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="E93" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="F93" t="n">
         <v>37.5628</v>
@@ -4720,14 +4741,14 @@
       <c r="I93" t="s">
         <v>85</v>
       </c>
-      <c r="J93" t="s">
-        <v>85</v>
+      <c r="J93" t="n">
+        <v>350.0</v>
       </c>
       <c r="K93" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="L93" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
     </row>
     <row r="94">
@@ -4741,10 +4762,10 @@
         <v>14</v>
       </c>
       <c r="D94" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="E94" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="F94" t="n">
         <v>38.2257</v>
@@ -4758,14 +4779,14 @@
       <c r="I94" t="s">
         <v>46</v>
       </c>
-      <c r="J94" t="s">
-        <v>46</v>
+      <c r="J94" t="n">
+        <v>150.0</v>
       </c>
       <c r="K94" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="L94" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
     </row>
     <row r="95">
@@ -4779,10 +4800,10 @@
         <v>14</v>
       </c>
       <c r="D95" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="E95" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="F95" t="n">
         <v>38.2257</v>
@@ -4796,14 +4817,14 @@
       <c r="I95" t="s">
         <v>46</v>
       </c>
-      <c r="J95" t="s">
-        <v>46</v>
+      <c r="J95" t="n">
+        <v>150.0</v>
       </c>
       <c r="K95" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="L95" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
     </row>
     <row r="96">
@@ -4817,10 +4838,10 @@
         <v>14</v>
       </c>
       <c r="D96" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="E96" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="F96" t="n">
         <v>39.0757</v>
@@ -4834,14 +4855,14 @@
       <c r="I96" t="s">
         <v>37</v>
       </c>
-      <c r="J96" t="s">
-        <v>37</v>
+      <c r="J96" t="n">
+        <v>325.0</v>
       </c>
       <c r="K96" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="L96" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="97">
@@ -4855,10 +4876,10 @@
         <v>14</v>
       </c>
       <c r="D97" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="E97" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="F97" t="n">
         <v>39.0757</v>
@@ -4870,16 +4891,16 @@
         <v>24</v>
       </c>
       <c r="I97" t="s">
-        <v>299</v>
-      </c>
-      <c r="J97" t="s">
-        <v>299</v>
+        <v>305</v>
+      </c>
+      <c r="J97" t="n">
+        <v>175.0</v>
       </c>
       <c r="K97" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="L97" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
     </row>
     <row r="98">
@@ -4893,10 +4914,10 @@
         <v>14</v>
       </c>
       <c r="D98" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="E98" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="F98" t="n">
         <v>40.4257</v>
@@ -4907,17 +4928,17 @@
       <c r="H98" t="s">
         <v>24</v>
       </c>
-      <c r="I98" t="n">
-        <v>208.0</v>
+      <c r="I98" t="s">
+        <v>309</v>
       </c>
       <c r="J98" t="n">
         <v>208.0</v>
       </c>
       <c r="K98" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="L98" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
     </row>
     <row r="99">
@@ -4931,10 +4952,10 @@
         <v>14</v>
       </c>
       <c r="D99" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="E99" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="F99" t="n">
         <v>39.752</v>
@@ -4952,10 +4973,10 @@
         <v>250.0</v>
       </c>
       <c r="K99" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="L99" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
     </row>
     <row r="100">
@@ -4969,10 +4990,10 @@
         <v>14</v>
       </c>
       <c r="D100" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="E100" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="F100" t="n">
         <v>39.957</v>
@@ -4986,14 +5007,14 @@
       <c r="I100" t="s">
         <v>37</v>
       </c>
-      <c r="J100" t="s">
-        <v>37</v>
+      <c r="J100" t="n">
+        <v>325.0</v>
       </c>
       <c r="K100" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="L100" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
     </row>
     <row r="101">
@@ -5001,16 +5022,16 @@
         <v>12</v>
       </c>
       <c r="B101" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="C101" t="s">
         <v>54</v>
       </c>
       <c r="D101" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="E101" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="F101" t="n">
         <v>40.1143</v>
@@ -5022,16 +5043,16 @@
         <v>62</v>
       </c>
       <c r="I101" t="s">
-        <v>313</v>
-      </c>
-      <c r="J101" t="s">
-        <v>313</v>
+        <v>320</v>
+      </c>
+      <c r="J101" t="n">
+        <v>350.0</v>
       </c>
       <c r="K101" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="L101" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="102">
@@ -5045,10 +5066,10 @@
         <v>50</v>
       </c>
       <c r="D102" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="E102" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="F102" t="n">
         <v>41.8574</v>
@@ -5060,16 +5081,16 @@
         <v>62</v>
       </c>
       <c r="I102" t="s">
-        <v>317</v>
-      </c>
-      <c r="J102" t="s">
-        <v>317</v>
+        <v>324</v>
+      </c>
+      <c r="J102" t="n">
+        <v>349.0</v>
       </c>
       <c r="K102" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="L102" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
     </row>
     <row r="103">
@@ -5083,10 +5104,10 @@
         <v>50</v>
       </c>
       <c r="D103" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E103" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F103" t="n">
         <v>42.025</v>
@@ -5095,19 +5116,19 @@
         <v>35.143</v>
       </c>
       <c r="H103" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="I103" t="s">
-        <v>323</v>
-      </c>
-      <c r="J103" t="s">
-        <v>323</v>
+        <v>330</v>
+      </c>
+      <c r="J103" t="n">
+        <v>450.0</v>
       </c>
       <c r="K103" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="L103" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
     </row>
     <row r="104">
@@ -5121,10 +5142,10 @@
         <v>50</v>
       </c>
       <c r="D104" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E104" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F104" t="n">
         <v>42.025</v>
@@ -5133,19 +5154,19 @@
         <v>35.143</v>
       </c>
       <c r="H104" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="I104" t="s">
-        <v>323</v>
-      </c>
-      <c r="J104" t="s">
-        <v>323</v>
+        <v>330</v>
+      </c>
+      <c r="J104" t="n">
+        <v>450.0</v>
       </c>
       <c r="K104" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="L104" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
     </row>
     <row r="105">
@@ -5159,10 +5180,10 @@
         <v>50</v>
       </c>
       <c r="D105" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E105" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F105" t="n">
         <v>42.025</v>
@@ -5176,14 +5197,14 @@
       <c r="I105" t="s">
         <v>62</v>
       </c>
-      <c r="J105" t="s">
-        <v>62</v>
+      <c r="J105" t="n">
+        <v>350.0</v>
       </c>
       <c r="K105" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="L105" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
     </row>
     <row r="106">
@@ -5197,10 +5218,10 @@
         <v>50</v>
       </c>
       <c r="D106" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E106" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F106" t="n">
         <v>42.025</v>
@@ -5212,16 +5233,16 @@
         <v>62</v>
       </c>
       <c r="I106" t="s">
-        <v>327</v>
-      </c>
-      <c r="J106" t="s">
-        <v>327</v>
+        <v>334</v>
+      </c>
+      <c r="J106" t="n">
+        <v>350.0</v>
       </c>
       <c r="K106" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="L106" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
     </row>
     <row r="107">
@@ -5235,10 +5256,10 @@
         <v>50</v>
       </c>
       <c r="D107" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E107" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F107" t="n">
         <v>42.025</v>
@@ -5250,16 +5271,16 @@
         <v>17</v>
       </c>
       <c r="I107" t="s">
-        <v>329</v>
-      </c>
-      <c r="J107" t="s">
-        <v>329</v>
+        <v>336</v>
+      </c>
+      <c r="J107" t="n">
+        <v>320.0</v>
       </c>
       <c r="K107" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="L107" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
     </row>
     <row r="108">
@@ -5273,10 +5294,10 @@
         <v>50</v>
       </c>
       <c r="D108" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E108" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F108" t="n">
         <v>42.025</v>
@@ -5290,14 +5311,14 @@
       <c r="I108" t="s">
         <v>85</v>
       </c>
-      <c r="J108" t="s">
-        <v>85</v>
+      <c r="J108" t="n">
+        <v>350.0</v>
       </c>
       <c r="K108" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="L108" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
     </row>
     <row r="109">
@@ -5311,10 +5332,10 @@
         <v>50</v>
       </c>
       <c r="D109" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E109" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F109" t="n">
         <v>42.025</v>
@@ -5328,14 +5349,14 @@
       <c r="I109" t="s">
         <v>85</v>
       </c>
-      <c r="J109" t="s">
-        <v>85</v>
+      <c r="J109" t="n">
+        <v>350.0</v>
       </c>
       <c r="K109" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="L109" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
     </row>
     <row r="110">
@@ -5349,10 +5370,10 @@
         <v>50</v>
       </c>
       <c r="D110" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E110" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F110" t="n">
         <v>42.025</v>
@@ -5366,14 +5387,14 @@
       <c r="I110" t="s">
         <v>51</v>
       </c>
-      <c r="J110" t="s">
-        <v>51</v>
+      <c r="J110" t="n">
+        <v>250.0</v>
       </c>
       <c r="K110" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="L110" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
     </row>
     <row r="111">
@@ -5387,10 +5408,10 @@
         <v>50</v>
       </c>
       <c r="D111" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E111" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F111" t="n">
         <v>42.025</v>
@@ -5402,16 +5423,16 @@
         <v>36</v>
       </c>
       <c r="I111" t="s">
-        <v>334</v>
-      </c>
-      <c r="J111" t="s">
-        <v>334</v>
+        <v>341</v>
+      </c>
+      <c r="J111" t="n">
+        <v>279.0</v>
       </c>
       <c r="K111" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="L111" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
     </row>
     <row r="112">
@@ -5425,10 +5446,10 @@
         <v>50</v>
       </c>
       <c r="D112" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E112" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F112" t="n">
         <v>42.025</v>
@@ -5440,16 +5461,16 @@
         <v>24</v>
       </c>
       <c r="I112" t="s">
-        <v>336</v>
-      </c>
-      <c r="J112" t="s">
-        <v>336</v>
+        <v>343</v>
+      </c>
+      <c r="J112" t="n">
+        <v>205.0</v>
       </c>
       <c r="K112" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="L112" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
     </row>
     <row r="113">
@@ -5463,10 +5484,10 @@
         <v>50</v>
       </c>
       <c r="D113" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E113" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F113" t="n">
         <v>42.025</v>
@@ -5475,19 +5496,19 @@
         <v>35.143</v>
       </c>
       <c r="H113" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="I113" t="s">
-        <v>338</v>
-      </c>
-      <c r="J113" t="s">
-        <v>338</v>
+        <v>345</v>
+      </c>
+      <c r="J113" t="n">
+        <v>450.0</v>
       </c>
       <c r="K113" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="L113" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
     </row>
     <row r="114">
@@ -5501,10 +5522,10 @@
         <v>14</v>
       </c>
       <c r="D114" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E114" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F114" t="n">
         <v>42.025</v>
@@ -5518,14 +5539,14 @@
       <c r="I114" t="s">
         <v>37</v>
       </c>
-      <c r="J114" t="s">
-        <v>37</v>
+      <c r="J114" t="n">
+        <v>325.0</v>
       </c>
       <c r="K114" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="L114" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
     </row>
     <row r="115">
@@ -5539,10 +5560,10 @@
         <v>50</v>
       </c>
       <c r="D115" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E115" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F115" t="n">
         <v>42.025</v>
@@ -5556,14 +5577,14 @@
       <c r="I115" t="s">
         <v>85</v>
       </c>
-      <c r="J115" t="s">
-        <v>85</v>
+      <c r="J115" t="n">
+        <v>350.0</v>
       </c>
       <c r="K115" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="L115" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
     </row>
     <row r="116">
@@ -5577,10 +5598,10 @@
         <v>50</v>
       </c>
       <c r="D116" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="E116" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="F116" t="n">
         <v>42.421</v>
@@ -5589,19 +5610,19 @@
         <v>27.693</v>
       </c>
       <c r="H116" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="I116" t="s">
-        <v>323</v>
-      </c>
-      <c r="J116" t="s">
-        <v>323</v>
+        <v>330</v>
+      </c>
+      <c r="J116" t="n">
+        <v>450.0</v>
       </c>
       <c r="K116" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="L116" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
     </row>
     <row r="117">
@@ -5609,16 +5630,16 @@
         <v>12</v>
       </c>
       <c r="B117" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="C117" t="s">
         <v>50</v>
       </c>
       <c r="D117" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="E117" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="F117" t="n">
         <v>42.421</v>
@@ -5627,19 +5648,19 @@
         <v>27.693</v>
       </c>
       <c r="H117" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="I117" t="s">
-        <v>323</v>
-      </c>
-      <c r="J117" t="s">
-        <v>323</v>
+        <v>330</v>
+      </c>
+      <c r="J117" t="n">
+        <v>450.0</v>
       </c>
       <c r="K117" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="L117" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
     </row>
     <row r="118">
@@ -5653,10 +5674,10 @@
         <v>14</v>
       </c>
       <c r="D118" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="E118" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="F118" t="n">
         <v>48.8148</v>
@@ -5670,14 +5691,14 @@
       <c r="I118" t="s">
         <v>51</v>
       </c>
-      <c r="J118" t="s">
-        <v>51</v>
+      <c r="J118" t="n">
+        <v>250.0</v>
       </c>
       <c r="K118" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="L118" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
     </row>
     <row r="119">
@@ -5691,10 +5712,10 @@
         <v>50</v>
       </c>
       <c r="D119" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="E119" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="F119" t="n">
         <v>48.547</v>
@@ -5708,14 +5729,14 @@
       <c r="I119" t="s">
         <v>24</v>
       </c>
-      <c r="J119" t="s">
-        <v>24</v>
+      <c r="J119" t="n">
+        <v>250.0</v>
       </c>
       <c r="K119" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="L119" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="120">
@@ -5729,10 +5750,10 @@
         <v>50</v>
       </c>
       <c r="D120" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="E120" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="F120" t="n">
         <v>48.547</v>
@@ -5746,14 +5767,14 @@
       <c r="I120" t="s">
         <v>24</v>
       </c>
-      <c r="J120" t="s">
-        <v>24</v>
+      <c r="J120" t="n">
+        <v>250.0</v>
       </c>
       <c r="K120" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="L120" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
     </row>
     <row r="121">
@@ -5767,10 +5788,10 @@
         <v>50</v>
       </c>
       <c r="D121" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="E121" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="F121" t="n">
         <v>48.547</v>
@@ -5784,31 +5805,31 @@
       <c r="I121" t="s">
         <v>51</v>
       </c>
-      <c r="J121" t="s">
-        <v>51</v>
+      <c r="J121" t="n">
+        <v>250.0</v>
       </c>
       <c r="K121" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="L121" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B122" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C122" t="s">
         <v>125</v>
       </c>
       <c r="D122" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="E122" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="F122" t="n">
         <v>48.547</v>
@@ -5822,14 +5843,14 @@
       <c r="I122" t="s">
         <v>62</v>
       </c>
-      <c r="J122" t="s">
-        <v>62</v>
+      <c r="J122" t="n">
+        <v>350.0</v>
       </c>
       <c r="K122" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="L122" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
     </row>
     <row r="123">
@@ -5843,10 +5864,10 @@
         <v>50</v>
       </c>
       <c r="D123" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="E123" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="F123" t="n">
         <v>45.1309</v>
@@ -5855,19 +5876,19 @@
         <v>36.4251</v>
       </c>
       <c r="H123" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="I123" t="s">
-        <v>360</v>
-      </c>
-      <c r="J123" t="s">
-        <v>360</v>
+        <v>367</v>
+      </c>
+      <c r="J123" t="n">
+        <v>399.0</v>
       </c>
       <c r="K123" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="L123" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
     </row>
     <row r="124">
@@ -5881,10 +5902,10 @@
         <v>14</v>
       </c>
       <c r="D124" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="E124" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="F124" t="n">
         <v>45.236</v>
@@ -5896,16 +5917,16 @@
         <v>17</v>
       </c>
       <c r="I124" t="s">
-        <v>365</v>
-      </c>
-      <c r="J124" t="s">
-        <v>365</v>
+        <v>372</v>
+      </c>
+      <c r="J124" t="n">
+        <v>299.0</v>
       </c>
       <c r="K124" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="L124" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
     </row>
     <row r="125">
@@ -5919,10 +5940,10 @@
         <v>50</v>
       </c>
       <c r="D125" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="E125" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="F125" t="n">
         <v>46.11</v>
@@ -5936,14 +5957,14 @@
       <c r="I125" t="s">
         <v>81</v>
       </c>
-      <c r="J125" t="s">
-        <v>81</v>
+      <c r="J125" t="n">
+        <v>375.0</v>
       </c>
       <c r="K125" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="L125" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
     </row>
     <row r="126">
@@ -5951,16 +5972,16 @@
         <v>12</v>
       </c>
       <c r="B126" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="C126" t="s">
         <v>54</v>
       </c>
       <c r="D126" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="E126" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="F126" t="n">
         <v>46.4133</v>
@@ -5974,14 +5995,14 @@
       <c r="I126" t="s">
         <v>51</v>
       </c>
-      <c r="J126" t="s">
-        <v>51</v>
+      <c r="J126" t="n">
+        <v>250.0</v>
       </c>
       <c r="K126" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="L126" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
     </row>
     <row r="127">
@@ -5995,10 +6016,10 @@
         <v>50</v>
       </c>
       <c r="D127" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="E127" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="F127" t="n">
         <v>46.4133</v>
@@ -6012,14 +6033,14 @@
       <c r="I127" t="s">
         <v>135</v>
       </c>
-      <c r="J127" t="s">
-        <v>135</v>
+      <c r="J127" t="n">
+        <v>450.0</v>
       </c>
       <c r="K127" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="L127" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
     </row>
     <row r="128">
@@ -6033,10 +6054,10 @@
         <v>50</v>
       </c>
       <c r="D128" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="E128" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="F128" t="n">
         <v>46.4133</v>
@@ -6050,14 +6071,14 @@
       <c r="I128" t="s">
         <v>24</v>
       </c>
-      <c r="J128" t="s">
-        <v>24</v>
+      <c r="J128" t="n">
+        <v>250.0</v>
       </c>
       <c r="K128" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="L128" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>